<commit_message>
Added Getting Address API Call Added Getting Currency API Call Added "02 Preparing Sales List Table" Flow within Preprocessing
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blast\Documents\UiPath\Relatorio_Vendas_GlobalIT_Nu\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35ADD410-F601-45D6-A9C8-9700FDF9B6B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B1156ED-B491-4F8D-ACC8-8A9D67C81992}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-35565" yWindow="1920" windowWidth="28800" windowHeight="11775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
   <si>
     <t>Name</t>
   </si>
@@ -154,13 +154,25 @@
   </si>
   <si>
     <t>Data\Input\Sales List.pdf</t>
+  </si>
+  <si>
+    <t>ViaCEP_API</t>
+  </si>
+  <si>
+    <t>https://viacep.com.br/ws/CEP/json/</t>
+  </si>
+  <si>
+    <t>AwesomeCurrency_API</t>
+  </si>
+  <si>
+    <t>https://economia.awesomeapi.com.br/json/last/Currency1-Currency2?token=CurrencyAPI</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -179,6 +191,13 @@
       <charset val="128"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -205,7 +224,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -215,6 +234,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -532,7 +554,7 @@
   <dimension ref="A1:Z995"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -596,9 +618,25 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A5" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" s="6"/>
+    </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>